<commit_message>
plano de negocio update
</commit_message>
<xml_diff>
--- a/Documentos/Proposta tecnica e financeira/Plano Negocio 1.0.xlsx
+++ b/Documentos/Proposta tecnica e financeira/Plano Negocio 1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8715" tabRatio="452"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8715" tabRatio="452" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Custo de Pessoal" sheetId="1" r:id="rId1"/>
@@ -412,41 +412,6 @@
   <dxfs count="39">
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
@@ -480,6 +445,41 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -730,15 +730,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="C3:Y24" totalsRowShown="0">
   <autoFilter ref="C3:Y24"/>
   <tableColumns count="23">
-    <tableColumn id="1" name="codigo" dataDxfId="14"/>
-    <tableColumn id="2" name="Processo" dataDxfId="13"/>
-    <tableColumn id="3" name="1 Semana" dataDxfId="12"/>
-    <tableColumn id="4" name="2 Semana" dataDxfId="11"/>
-    <tableColumn id="5" name="3 Semana" dataDxfId="10"/>
-    <tableColumn id="6" name="4 Semana" dataDxfId="9"/>
-    <tableColumn id="7" name="5 Semana" dataDxfId="8"/>
-    <tableColumn id="8" name="6 Semana" dataDxfId="7"/>
-    <tableColumn id="9" name="7 Semana" dataDxfId="6"/>
+    <tableColumn id="1" name="codigo" dataDxfId="9"/>
+    <tableColumn id="2" name="Processo" dataDxfId="8"/>
+    <tableColumn id="3" name="1 Semana" dataDxfId="7"/>
+    <tableColumn id="4" name="2 Semana" dataDxfId="6"/>
+    <tableColumn id="5" name="3 Semana" dataDxfId="5"/>
+    <tableColumn id="6" name="4 Semana" dataDxfId="4"/>
+    <tableColumn id="7" name="5 Semana" dataDxfId="3"/>
+    <tableColumn id="8" name="6 Semana" dataDxfId="2"/>
+    <tableColumn id="9" name="7 Semana" dataDxfId="1"/>
     <tableColumn id="10" name="8 Semana"/>
     <tableColumn id="11" name="9 Semana"/>
     <tableColumn id="12" name="10 Semana"/>
@@ -752,7 +752,7 @@
     <tableColumn id="21" name="18 Semana"/>
     <tableColumn id="22" name="19 Semana"/>
     <tableColumn id="23" name="20 Semana"/>
-    <tableColumn id="17" name="21 Semana" dataDxfId="5"/>
+    <tableColumn id="17" name="21 Semana" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1047,7 +1047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+    <sheetView topLeftCell="A38" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -2115,6 +2115,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B20:G20"/>
     <mergeCell ref="B51:G51"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B30:C30"/>
@@ -2122,11 +2127,6 @@
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B42:G42"/>
     <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2145,7 +2145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:Y33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
@@ -2649,21 +2649,21 @@
     <mergeCell ref="J1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E33:X1048576 E32:G32 I32:X32 E1:X5 E25:X31 E6:E24 G6:Y24">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:X5 E6:E24 G6:Y24">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>